<commit_message>
Update: LoRa distance test 4 5
</commit_message>
<xml_diff>
--- a/Documents/LoRaDistanceTest/TestResultSummary.xlsx
+++ b/Documents/LoRaDistanceTest/TestResultSummary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thao Nguyen\Desktop\Files\LoRa Test Result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\KLTN-WeatherForecast\Documents\LoRaDistanceTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4186FD0-062D-44B3-A267-86C2A2D799DC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9B8A85-D1A2-4EB8-B442-603736A8E775}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{746FF340-C7F6-4D65-9FEE-A5E7FAEFF6CA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Test No.</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Packet error</t>
+  </si>
+  <si>
+    <t>135.75m</t>
+  </si>
+  <si>
+    <t>73.42m</t>
   </si>
 </sst>
 </file>
@@ -122,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -137,6 +143,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052AB242-BC80-40B4-8B80-36E527500DB1}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -560,6 +569,61 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>43299</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>144</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>43299</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>81</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>